<commit_message>
- Stripped lines with no "To" field. - Stripped the ID part of the message ID and only keep the server. - Added auto-zip functionality. - Added Message-ID to feature analysis
</commit_message>
<xml_diff>
--- a/feature_analysis/output/feature_analysis.xlsx
+++ b/feature_analysis/output/feature_analysis.xlsx
@@ -15,13 +15,14 @@
     <sheet name="ContentType" sheetId="6" r:id="rId6"/>
     <sheet name="MimeType" sheetId="7" r:id="rId7"/>
     <sheet name="TransferEncoding" sheetId="8" r:id="rId8"/>
+    <sheet name="MessageID" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="189">
   <si>
     <t>User</t>
   </si>
@@ -567,6 +568,9 @@
   </si>
   <si>
     <t>base64</t>
+  </si>
+  <si>
+    <t>thyme</t>
   </si>
   <si>
     <t>Max Sent</t>
@@ -3216,6 +3220,97 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" baseline="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
+              <a:t>Number of emails of each Message-ID</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MessageID!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>MessageID!$A$2:$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>thyme</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MessageID!$B$2:$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>517401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3425,6 +3520,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3739,7 +3864,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B1">
         <f>MAX(SentEmailCounts!$B$2:$B$147)</f>
@@ -3748,7 +3873,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <f>MIN(SentEmailCounts!$B$2:$B$147)</f>
@@ -3757,7 +3882,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <f>AVERAGE(SentEmailCounts!$B$2:$B$147)</f>
@@ -3766,7 +3891,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B5">
         <f>MAX(ReceivedEmailCounts!$B$2:$B$147)</f>
@@ -3775,7 +3900,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B6">
         <f>MIN(ReceivedEmailCounts!$B$2:$B$147)</f>
@@ -3784,7 +3909,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B7">
         <f>AVERAGE(SentEmailCounts!$B$2:$B$147)</f>
@@ -6511,4 +6636,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2">
+        <v>517401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed anonymization of feature analysis.
</commit_message>
<xml_diff>
--- a/feature_analysis/output/feature_analysis.xlsx
+++ b/feature_analysis/output/feature_analysis.xlsx
@@ -1129,442 +1129,442 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="146"/>
                 <c:pt idx="0">
-                  <c:v>2195</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3578</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>201</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5158</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>309</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>363</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1210</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>480</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1053</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1388</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>721</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1824</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>527</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>940</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>169</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>275</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11411</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>899</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>101</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3069</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>909</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>448</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>380</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>76</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1840</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>57</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2812</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>91</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>450</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3706</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>108</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>526</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>770</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8801</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>136</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2963</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1719</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>970</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1941</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1456</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1061</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1061</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>133</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>888</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>196</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1073</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>821</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1454</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>8490</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>14368</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6759</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>263</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>587</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1728</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>810</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2990</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>36</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5265</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>133</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>904</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>157</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3112</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>335</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>772</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>16735</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>230</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>185</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>215</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2742</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>217</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1325</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>47</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>212</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1829</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>3888</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>675</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>566</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>417</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4387</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>675</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>83</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>130</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>885</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>260</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>605</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>184</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>84</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>376</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>473</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2496</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>3427</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>631</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2636</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>44</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>3262</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>325</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>624</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>255</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>4000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>736</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>8777</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2681</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1215</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1052</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>108</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1060</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>146</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>181</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>3564</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1655</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>105</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>532</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>176</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>186</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>5438</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>4111</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>767</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>163</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>167</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>732</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>410</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>1217</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>117</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>556</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>556</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>501</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="139">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>223</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>716</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>110</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>252</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>352</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2144,442 +2144,442 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="146"/>
                 <c:pt idx="0">
-                  <c:v>3375</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3541</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1790</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3931</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3066</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4404</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1541</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2612</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2482</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1243</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4026</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2555</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2539</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2558</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6746</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4044</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2406</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1229</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16666</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4072</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2593</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3506</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2457</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2888</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3377</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1560</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2089</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6784</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1083</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1294</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2335</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>935</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1486</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5032</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3270</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>816</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4450</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11599</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4687</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4988</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>135</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3169</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3469</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1392</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>992</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4368</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3278</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2705</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3443</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2734</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15221</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6850</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>16033</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>885</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2969</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2607</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>9479</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1756</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>8682</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4609</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3581</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1243</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5554</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4128</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1268</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1482</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>698</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2616</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7878</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1631</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1730</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1688</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>3794</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2365</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2414</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2948</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>3141</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>3341</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1307</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1928</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4460</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>7778</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4416</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1673</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>888</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2923</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4416</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1747</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2313</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3013</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1670</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2448</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>573</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2141</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>612</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>694</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>5292</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1892</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>6958</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2390</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2772</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>5413</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2524</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1752</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1814</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>3796</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1856</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>14099</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>3832</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>18917</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1840</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3945</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>10188</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1371</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>10306</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>793</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>556</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>4341</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>3532</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>3154</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1185</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>3012</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2147</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>2512</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>6308</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>12902</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1096</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1836</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>2942</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>3026</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>1619</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>4016</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>723</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>6656</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>6656</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>2153</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>51</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>1290</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>5793</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>2354</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>1841</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>3205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>875</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3942,7 +3942,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3950,7 +3950,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>3578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3958,7 +3958,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3966,7 +3966,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3974,7 +3974,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>5158</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3982,7 +3982,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>309</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3990,7 +3990,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3998,7 +3998,7 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4006,7 +4006,7 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>1210</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4014,7 +4014,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>480</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4022,7 +4022,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>1053</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4030,7 +4030,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>1388</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4038,7 +4038,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>721</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4046,7 +4046,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>1824</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4054,7 +4054,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>527</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4062,7 +4062,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>940</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4070,7 +4070,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>169</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4078,7 +4078,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4086,7 +4086,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>11411</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4094,7 +4094,7 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4102,7 +4102,7 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4110,7 +4110,7 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>3069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4118,7 +4118,7 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>909</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4126,7 +4126,7 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4134,7 +4134,7 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>380</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4142,7 +4142,7 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4150,7 +4150,7 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>1840</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4158,7 +4158,7 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4166,7 +4166,7 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>2812</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4174,7 +4174,7 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4182,7 +4182,7 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>450</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4190,7 +4190,7 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>3706</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4198,7 +4198,7 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4206,7 +4206,7 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>526</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4214,7 +4214,7 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>770</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4222,7 +4222,7 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>8801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4230,7 +4230,7 @@
         <v>42</v>
       </c>
       <c r="B38">
-        <v>136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4238,7 +4238,7 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>2963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4246,7 +4246,7 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>1719</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4254,7 +4254,7 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>970</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4262,7 +4262,7 @@
         <v>46</v>
       </c>
       <c r="B42">
-        <v>1941</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4270,7 +4270,7 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>1456</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4286,7 +4286,7 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>1061</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4294,7 +4294,7 @@
         <v>50</v>
       </c>
       <c r="B46">
-        <v>1061</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4302,7 +4302,7 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>133</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4310,7 +4310,7 @@
         <v>52</v>
       </c>
       <c r="B48">
-        <v>888</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4318,7 +4318,7 @@
         <v>53</v>
       </c>
       <c r="B49">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4326,7 +4326,7 @@
         <v>54</v>
       </c>
       <c r="B50">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4334,7 +4334,7 @@
         <v>55</v>
       </c>
       <c r="B51">
-        <v>1073</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4342,7 +4342,7 @@
         <v>56</v>
       </c>
       <c r="B52">
-        <v>821</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4350,7 +4350,7 @@
         <v>57</v>
       </c>
       <c r="B53">
-        <v>1454</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4358,7 +4358,7 @@
         <v>58</v>
       </c>
       <c r="B54">
-        <v>8490</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4366,7 +4366,7 @@
         <v>59</v>
       </c>
       <c r="B55">
-        <v>14368</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4374,7 +4374,7 @@
         <v>60</v>
       </c>
       <c r="B56">
-        <v>6759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4382,7 +4382,7 @@
         <v>61</v>
       </c>
       <c r="B57">
-        <v>263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4390,7 +4390,7 @@
         <v>62</v>
       </c>
       <c r="B58">
-        <v>587</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -4398,7 +4398,7 @@
         <v>63</v>
       </c>
       <c r="B59">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4406,7 +4406,7 @@
         <v>64</v>
       </c>
       <c r="B60">
-        <v>1728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4414,7 +4414,7 @@
         <v>65</v>
       </c>
       <c r="B61">
-        <v>810</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4422,7 +4422,7 @@
         <v>66</v>
       </c>
       <c r="B62">
-        <v>2990</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -4430,7 +4430,7 @@
         <v>67</v>
       </c>
       <c r="B63">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4438,7 +4438,7 @@
         <v>68</v>
       </c>
       <c r="B64">
-        <v>5265</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4446,7 +4446,7 @@
         <v>69</v>
       </c>
       <c r="B65">
-        <v>133</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4454,7 +4454,7 @@
         <v>70</v>
       </c>
       <c r="B66">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4462,7 +4462,7 @@
         <v>71</v>
       </c>
       <c r="B67">
-        <v>904</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4470,7 +4470,7 @@
         <v>72</v>
       </c>
       <c r="B68">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4478,7 +4478,7 @@
         <v>73</v>
       </c>
       <c r="B69">
-        <v>3112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4486,7 +4486,7 @@
         <v>74</v>
       </c>
       <c r="B70">
-        <v>335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4494,7 +4494,7 @@
         <v>75</v>
       </c>
       <c r="B71">
-        <v>772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4502,7 +4502,7 @@
         <v>76</v>
       </c>
       <c r="B72">
-        <v>16735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -4510,7 +4510,7 @@
         <v>77</v>
       </c>
       <c r="B73">
-        <v>230</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -4518,7 +4518,7 @@
         <v>78</v>
       </c>
       <c r="B74">
-        <v>185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -4526,7 +4526,7 @@
         <v>79</v>
       </c>
       <c r="B75">
-        <v>215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -4534,7 +4534,7 @@
         <v>80</v>
       </c>
       <c r="B76">
-        <v>2742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -4542,7 +4542,7 @@
         <v>81</v>
       </c>
       <c r="B77">
-        <v>217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -4550,7 +4550,7 @@
         <v>82</v>
       </c>
       <c r="B78">
-        <v>333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -4558,7 +4558,7 @@
         <v>83</v>
       </c>
       <c r="B79">
-        <v>1325</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -4566,7 +4566,7 @@
         <v>84</v>
       </c>
       <c r="B80">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -4574,7 +4574,7 @@
         <v>85</v>
       </c>
       <c r="B81">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -4582,7 +4582,7 @@
         <v>86</v>
       </c>
       <c r="B82">
-        <v>212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -4590,7 +4590,7 @@
         <v>87</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -4598,7 +4598,7 @@
         <v>88</v>
       </c>
       <c r="B84">
-        <v>1829</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -4606,7 +4606,7 @@
         <v>89</v>
       </c>
       <c r="B85">
-        <v>3888</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -4614,7 +4614,7 @@
         <v>90</v>
       </c>
       <c r="B86">
-        <v>675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -4622,7 +4622,7 @@
         <v>91</v>
       </c>
       <c r="B87">
-        <v>566</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -4630,7 +4630,7 @@
         <v>92</v>
       </c>
       <c r="B88">
-        <v>417</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -4638,7 +4638,7 @@
         <v>93</v>
       </c>
       <c r="B89">
-        <v>4387</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -4646,7 +4646,7 @@
         <v>94</v>
       </c>
       <c r="B90">
-        <v>675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -4654,7 +4654,7 @@
         <v>95</v>
       </c>
       <c r="B91">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -4662,7 +4662,7 @@
         <v>96</v>
       </c>
       <c r="B92">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -4670,7 +4670,7 @@
         <v>97</v>
       </c>
       <c r="B93">
-        <v>885</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -4678,7 +4678,7 @@
         <v>98</v>
       </c>
       <c r="B94">
-        <v>260</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -4686,7 +4686,7 @@
         <v>99</v>
       </c>
       <c r="B95">
-        <v>605</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -4694,7 +4694,7 @@
         <v>100</v>
       </c>
       <c r="B96">
-        <v>184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -4702,7 +4702,7 @@
         <v>101</v>
       </c>
       <c r="B97">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -4710,7 +4710,7 @@
         <v>102</v>
       </c>
       <c r="B98">
-        <v>376</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -4718,7 +4718,7 @@
         <v>103</v>
       </c>
       <c r="B99">
-        <v>473</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -4726,7 +4726,7 @@
         <v>104</v>
       </c>
       <c r="B100">
-        <v>2496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -4734,7 +4734,7 @@
         <v>105</v>
       </c>
       <c r="B101">
-        <v>3427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -4742,7 +4742,7 @@
         <v>106</v>
       </c>
       <c r="B102">
-        <v>631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -4750,7 +4750,7 @@
         <v>107</v>
       </c>
       <c r="B103">
-        <v>2636</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -4758,7 +4758,7 @@
         <v>108</v>
       </c>
       <c r="B104">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -4766,7 +4766,7 @@
         <v>109</v>
       </c>
       <c r="B105">
-        <v>182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -4774,7 +4774,7 @@
         <v>110</v>
       </c>
       <c r="B106">
-        <v>3262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -4782,7 +4782,7 @@
         <v>111</v>
       </c>
       <c r="B107">
-        <v>325</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -4790,7 +4790,7 @@
         <v>112</v>
       </c>
       <c r="B108">
-        <v>624</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -4798,7 +4798,7 @@
         <v>113</v>
       </c>
       <c r="B109">
-        <v>255</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -4806,7 +4806,7 @@
         <v>114</v>
       </c>
       <c r="B110">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -4814,7 +4814,7 @@
         <v>115</v>
       </c>
       <c r="B111">
-        <v>736</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -4822,7 +4822,7 @@
         <v>116</v>
       </c>
       <c r="B112">
-        <v>8777</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -4830,7 +4830,7 @@
         <v>117</v>
       </c>
       <c r="B113">
-        <v>2681</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -4838,7 +4838,7 @@
         <v>118</v>
       </c>
       <c r="B114">
-        <v>1215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -4846,7 +4846,7 @@
         <v>119</v>
       </c>
       <c r="B115">
-        <v>1052</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -4854,7 +4854,7 @@
         <v>120</v>
       </c>
       <c r="B116">
-        <v>108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -4862,7 +4862,7 @@
         <v>121</v>
       </c>
       <c r="B117">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -4870,7 +4870,7 @@
         <v>122</v>
       </c>
       <c r="B118">
-        <v>1060</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -4878,7 +4878,7 @@
         <v>123</v>
       </c>
       <c r="B119">
-        <v>146</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -4886,7 +4886,7 @@
         <v>124</v>
       </c>
       <c r="B120">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -4894,7 +4894,7 @@
         <v>125</v>
       </c>
       <c r="B121">
-        <v>181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -4902,7 +4902,7 @@
         <v>126</v>
       </c>
       <c r="B122">
-        <v>3564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -4910,7 +4910,7 @@
         <v>127</v>
       </c>
       <c r="B123">
-        <v>1655</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -4918,7 +4918,7 @@
         <v>128</v>
       </c>
       <c r="B124">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -4926,7 +4926,7 @@
         <v>129</v>
       </c>
       <c r="B125">
-        <v>532</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -4934,7 +4934,7 @@
         <v>130</v>
       </c>
       <c r="B126">
-        <v>176</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -4942,7 +4942,7 @@
         <v>131</v>
       </c>
       <c r="B127">
-        <v>186</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -4950,7 +4950,7 @@
         <v>132</v>
       </c>
       <c r="B128">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -4958,7 +4958,7 @@
         <v>133</v>
       </c>
       <c r="B129">
-        <v>5438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -4966,7 +4966,7 @@
         <v>134</v>
       </c>
       <c r="B130">
-        <v>4111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -4974,7 +4974,7 @@
         <v>135</v>
       </c>
       <c r="B131">
-        <v>767</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -4982,7 +4982,7 @@
         <v>136</v>
       </c>
       <c r="B132">
-        <v>163</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -4990,7 +4990,7 @@
         <v>137</v>
       </c>
       <c r="B133">
-        <v>167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -4998,7 +4998,7 @@
         <v>138</v>
       </c>
       <c r="B134">
-        <v>732</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -5006,7 +5006,7 @@
         <v>139</v>
       </c>
       <c r="B135">
-        <v>410</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -5014,7 +5014,7 @@
         <v>140</v>
       </c>
       <c r="B136">
-        <v>1217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -5022,7 +5022,7 @@
         <v>141</v>
       </c>
       <c r="B137">
-        <v>117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -5030,7 +5030,7 @@
         <v>142</v>
       </c>
       <c r="B138">
-        <v>556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -5038,7 +5038,7 @@
         <v>143</v>
       </c>
       <c r="B139">
-        <v>556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -5046,7 +5046,7 @@
         <v>144</v>
       </c>
       <c r="B140">
-        <v>501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -5062,7 +5062,7 @@
         <v>146</v>
       </c>
       <c r="B142">
-        <v>223</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -5070,7 +5070,7 @@
         <v>147</v>
       </c>
       <c r="B143">
-        <v>716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -5078,7 +5078,7 @@
         <v>148</v>
       </c>
       <c r="B144">
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -5086,7 +5086,7 @@
         <v>149</v>
       </c>
       <c r="B145">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -5094,7 +5094,7 @@
         <v>150</v>
       </c>
       <c r="B146">
-        <v>497</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -5102,7 +5102,7 @@
         <v>151</v>
       </c>
       <c r="B147">
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5131,7 +5131,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>3375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5139,7 +5139,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>3541</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5147,7 +5147,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>1790</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5155,7 +5155,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>3931</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5163,7 +5163,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>3066</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5171,7 +5171,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>4404</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5179,7 +5179,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>1541</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5187,7 +5187,7 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>2612</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5195,7 +5195,7 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>2482</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5203,7 +5203,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>1243</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5211,7 +5211,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>4026</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5219,7 +5219,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>2555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5227,7 +5227,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>2539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5235,7 +5235,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>2558</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -5243,7 +5243,7 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>6746</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5251,7 +5251,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>4044</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -5259,7 +5259,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>2406</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5267,7 +5267,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>1229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5275,7 +5275,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>16666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -5283,7 +5283,7 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>4072</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5291,7 +5291,7 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>2593</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5299,7 +5299,7 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>3506</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -5307,7 +5307,7 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>2457</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -5315,7 +5315,7 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>2888</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5323,7 +5323,7 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>3377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -5331,7 +5331,7 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>1451</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5339,7 +5339,7 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>1560</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5347,7 +5347,7 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>2089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -5355,7 +5355,7 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>6784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -5363,7 +5363,7 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>1083</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -5371,7 +5371,7 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>1294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -5379,7 +5379,7 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>2335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5387,7 +5387,7 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>935</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -5395,7 +5395,7 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -5403,7 +5403,7 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>1486</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5411,7 +5411,7 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>5032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -5419,7 +5419,7 @@
         <v>42</v>
       </c>
       <c r="B38">
-        <v>3270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5427,7 +5427,7 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>816</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -5435,7 +5435,7 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>4450</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -5443,7 +5443,7 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>11599</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -5451,7 +5451,7 @@
         <v>46</v>
       </c>
       <c r="B42">
-        <v>4687</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -5459,7 +5459,7 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>4988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -5467,7 +5467,7 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -5475,7 +5475,7 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>3169</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -5483,7 +5483,7 @@
         <v>50</v>
       </c>
       <c r="B46">
-        <v>3469</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -5491,7 +5491,7 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>1392</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -5499,7 +5499,7 @@
         <v>52</v>
       </c>
       <c r="B48">
-        <v>992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -5507,7 +5507,7 @@
         <v>53</v>
       </c>
       <c r="B49">
-        <v>4368</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -5515,7 +5515,7 @@
         <v>54</v>
       </c>
       <c r="B50">
-        <v>3278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -5523,7 +5523,7 @@
         <v>55</v>
       </c>
       <c r="B51">
-        <v>2705</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -5531,7 +5531,7 @@
         <v>56</v>
       </c>
       <c r="B52">
-        <v>3443</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -5539,7 +5539,7 @@
         <v>57</v>
       </c>
       <c r="B53">
-        <v>2734</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -5547,7 +5547,7 @@
         <v>58</v>
       </c>
       <c r="B54">
-        <v>15221</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -5555,7 +5555,7 @@
         <v>59</v>
       </c>
       <c r="B55">
-        <v>6850</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5563,7 +5563,7 @@
         <v>60</v>
       </c>
       <c r="B56">
-        <v>16033</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -5571,7 +5571,7 @@
         <v>61</v>
       </c>
       <c r="B57">
-        <v>885</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -5579,7 +5579,7 @@
         <v>62</v>
       </c>
       <c r="B58">
-        <v>2969</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -5587,7 +5587,7 @@
         <v>63</v>
       </c>
       <c r="B59">
-        <v>2607</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -5595,7 +5595,7 @@
         <v>64</v>
       </c>
       <c r="B60">
-        <v>9479</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -5603,7 +5603,7 @@
         <v>65</v>
       </c>
       <c r="B61">
-        <v>1756</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -5611,7 +5611,7 @@
         <v>66</v>
       </c>
       <c r="B62">
-        <v>8682</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -5619,7 +5619,7 @@
         <v>67</v>
       </c>
       <c r="B63">
-        <v>4609</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5627,7 +5627,7 @@
         <v>68</v>
       </c>
       <c r="B64">
-        <v>3581</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -5635,7 +5635,7 @@
         <v>69</v>
       </c>
       <c r="B65">
-        <v>1243</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -5643,7 +5643,7 @@
         <v>70</v>
       </c>
       <c r="B66">
-        <v>5554</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -5651,7 +5651,7 @@
         <v>71</v>
       </c>
       <c r="B67">
-        <v>4128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -5659,7 +5659,7 @@
         <v>72</v>
       </c>
       <c r="B68">
-        <v>1268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -5667,7 +5667,7 @@
         <v>73</v>
       </c>
       <c r="B69">
-        <v>1482</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -5675,7 +5675,7 @@
         <v>74</v>
       </c>
       <c r="B70">
-        <v>698</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -5683,7 +5683,7 @@
         <v>75</v>
       </c>
       <c r="B71">
-        <v>2616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -5691,7 +5691,7 @@
         <v>76</v>
       </c>
       <c r="B72">
-        <v>7878</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -5699,7 +5699,7 @@
         <v>77</v>
       </c>
       <c r="B73">
-        <v>1631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -5707,7 +5707,7 @@
         <v>78</v>
       </c>
       <c r="B74">
-        <v>1730</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -5715,7 +5715,7 @@
         <v>79</v>
       </c>
       <c r="B75">
-        <v>1688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -5723,7 +5723,7 @@
         <v>80</v>
       </c>
       <c r="B76">
-        <v>3794</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -5731,7 +5731,7 @@
         <v>81</v>
       </c>
       <c r="B77">
-        <v>2365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -5739,7 +5739,7 @@
         <v>82</v>
       </c>
       <c r="B78">
-        <v>2414</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -5747,7 +5747,7 @@
         <v>83</v>
       </c>
       <c r="B79">
-        <v>2948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -5755,7 +5755,7 @@
         <v>84</v>
       </c>
       <c r="B80">
-        <v>3141</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -5763,7 +5763,7 @@
         <v>85</v>
       </c>
       <c r="B81">
-        <v>3341</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -5771,7 +5771,7 @@
         <v>86</v>
       </c>
       <c r="B82">
-        <v>1307</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -5779,7 +5779,7 @@
         <v>87</v>
       </c>
       <c r="B83">
-        <v>1928</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -5787,7 +5787,7 @@
         <v>88</v>
       </c>
       <c r="B84">
-        <v>4460</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -5795,7 +5795,7 @@
         <v>89</v>
       </c>
       <c r="B85">
-        <v>7778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -5803,7 +5803,7 @@
         <v>90</v>
       </c>
       <c r="B86">
-        <v>4416</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -5811,7 +5811,7 @@
         <v>91</v>
       </c>
       <c r="B87">
-        <v>1673</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -5819,7 +5819,7 @@
         <v>92</v>
       </c>
       <c r="B88">
-        <v>888</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -5827,7 +5827,7 @@
         <v>93</v>
       </c>
       <c r="B89">
-        <v>2923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -5835,7 +5835,7 @@
         <v>94</v>
       </c>
       <c r="B90">
-        <v>4416</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -5843,7 +5843,7 @@
         <v>95</v>
       </c>
       <c r="B91">
-        <v>1747</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -5851,7 +5851,7 @@
         <v>96</v>
       </c>
       <c r="B92">
-        <v>2313</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -5859,7 +5859,7 @@
         <v>97</v>
       </c>
       <c r="B93">
-        <v>3013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -5867,7 +5867,7 @@
         <v>98</v>
       </c>
       <c r="B94">
-        <v>1670</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -5875,7 +5875,7 @@
         <v>99</v>
       </c>
       <c r="B95">
-        <v>2448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -5883,7 +5883,7 @@
         <v>100</v>
       </c>
       <c r="B96">
-        <v>573</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -5891,7 +5891,7 @@
         <v>101</v>
       </c>
       <c r="B97">
-        <v>2141</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -5899,7 +5899,7 @@
         <v>102</v>
       </c>
       <c r="B98">
-        <v>612</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -5907,7 +5907,7 @@
         <v>103</v>
       </c>
       <c r="B99">
-        <v>2333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -5915,7 +5915,7 @@
         <v>104</v>
       </c>
       <c r="B100">
-        <v>694</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -5923,7 +5923,7 @@
         <v>105</v>
       </c>
       <c r="B101">
-        <v>5292</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -5931,7 +5931,7 @@
         <v>106</v>
       </c>
       <c r="B102">
-        <v>1892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -5939,7 +5939,7 @@
         <v>107</v>
       </c>
       <c r="B103">
-        <v>6958</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -5947,7 +5947,7 @@
         <v>108</v>
       </c>
       <c r="B104">
-        <v>2390</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -5955,7 +5955,7 @@
         <v>109</v>
       </c>
       <c r="B105">
-        <v>2772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -5963,7 +5963,7 @@
         <v>110</v>
       </c>
       <c r="B106">
-        <v>5413</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -5971,7 +5971,7 @@
         <v>111</v>
       </c>
       <c r="B107">
-        <v>2524</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -5979,7 +5979,7 @@
         <v>112</v>
       </c>
       <c r="B108">
-        <v>1752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -5987,7 +5987,7 @@
         <v>113</v>
       </c>
       <c r="B109">
-        <v>1814</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -5995,7 +5995,7 @@
         <v>114</v>
       </c>
       <c r="B110">
-        <v>3796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -6003,7 +6003,7 @@
         <v>115</v>
       </c>
       <c r="B111">
-        <v>1856</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -6011,7 +6011,7 @@
         <v>116</v>
       </c>
       <c r="B112">
-        <v>14099</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -6019,7 +6019,7 @@
         <v>117</v>
       </c>
       <c r="B113">
-        <v>3832</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -6027,7 +6027,7 @@
         <v>118</v>
       </c>
       <c r="B114">
-        <v>18917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -6035,7 +6035,7 @@
         <v>119</v>
       </c>
       <c r="B115">
-        <v>1840</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -6043,7 +6043,7 @@
         <v>120</v>
       </c>
       <c r="B116">
-        <v>3945</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -6051,7 +6051,7 @@
         <v>121</v>
       </c>
       <c r="B117">
-        <v>10188</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -6059,7 +6059,7 @@
         <v>122</v>
       </c>
       <c r="B118">
-        <v>1371</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -6067,7 +6067,7 @@
         <v>123</v>
       </c>
       <c r="B119">
-        <v>10306</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -6075,7 +6075,7 @@
         <v>124</v>
       </c>
       <c r="B120">
-        <v>793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -6083,7 +6083,7 @@
         <v>125</v>
       </c>
       <c r="B121">
-        <v>556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -6091,7 +6091,7 @@
         <v>126</v>
       </c>
       <c r="B122">
-        <v>4341</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -6099,7 +6099,7 @@
         <v>127</v>
       </c>
       <c r="B123">
-        <v>3532</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -6107,7 +6107,7 @@
         <v>128</v>
       </c>
       <c r="B124">
-        <v>3154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -6115,7 +6115,7 @@
         <v>129</v>
       </c>
       <c r="B125">
-        <v>1185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -6123,7 +6123,7 @@
         <v>130</v>
       </c>
       <c r="B126">
-        <v>3012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -6131,7 +6131,7 @@
         <v>131</v>
       </c>
       <c r="B127">
-        <v>2147</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -6139,7 +6139,7 @@
         <v>132</v>
       </c>
       <c r="B128">
-        <v>2512</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -6147,7 +6147,7 @@
         <v>133</v>
       </c>
       <c r="B129">
-        <v>6308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -6155,7 +6155,7 @@
         <v>134</v>
       </c>
       <c r="B130">
-        <v>12902</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -6163,7 +6163,7 @@
         <v>135</v>
       </c>
       <c r="B131">
-        <v>1096</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -6171,7 +6171,7 @@
         <v>136</v>
       </c>
       <c r="B132">
-        <v>1836</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -6179,7 +6179,7 @@
         <v>137</v>
       </c>
       <c r="B133">
-        <v>2942</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -6187,7 +6187,7 @@
         <v>138</v>
       </c>
       <c r="B134">
-        <v>3026</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -6195,7 +6195,7 @@
         <v>139</v>
       </c>
       <c r="B135">
-        <v>1619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -6203,7 +6203,7 @@
         <v>140</v>
       </c>
       <c r="B136">
-        <v>4016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -6211,7 +6211,7 @@
         <v>141</v>
       </c>
       <c r="B137">
-        <v>723</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -6219,7 +6219,7 @@
         <v>142</v>
       </c>
       <c r="B138">
-        <v>6656</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -6227,7 +6227,7 @@
         <v>143</v>
       </c>
       <c r="B139">
-        <v>6656</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -6235,7 +6235,7 @@
         <v>144</v>
       </c>
       <c r="B140">
-        <v>2153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -6243,7 +6243,7 @@
         <v>145</v>
       </c>
       <c r="B141">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -6251,7 +6251,7 @@
         <v>146</v>
       </c>
       <c r="B142">
-        <v>1290</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -6259,7 +6259,7 @@
         <v>147</v>
       </c>
       <c r="B143">
-        <v>5793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -6267,7 +6267,7 @@
         <v>148</v>
       </c>
       <c r="B144">
-        <v>2354</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -6275,7 +6275,7 @@
         <v>149</v>
       </c>
       <c r="B145">
-        <v>1841</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -6283,7 +6283,7 @@
         <v>150</v>
       </c>
       <c r="B146">
-        <v>3205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -6291,7 +6291,7 @@
         <v>151</v>
       </c>
       <c r="B147">
-        <v>875</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>